<commit_message>
Trained the CNN on more fillers vs. non-fillers data, added familiar exercise phrase keywords, improved keyword highlighting in web tool
</commit_message>
<xml_diff>
--- a/Keyword Extraction/Results_Detailed Accuracy/detailedAccuracy_Output.txt.xlsx
+++ b/Keyword Extraction/Results_Detailed Accuracy/detailedAccuracy_Output.txt.xlsx
@@ -1094,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>99.99955892562866</v>
+        <v>99.99992847442627</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1124,10 +1124,10 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>99.62270259857178</v>
+        <v>99.9825656414032</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1135,10 +1135,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>99.99997615814209</v>
+        <v>60.59531569480896</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1149,7 +1149,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1157,10 +1157,10 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>85.95828413963318</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1168,7 +1168,7 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>100</v>
@@ -1179,10 +1179,10 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>99.96410608291626</v>
+        <v>91.99870824813843</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1215,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>99.99985694885254</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1226,7 +1226,7 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1237,7 +1237,7 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>88.06438446044922</v>
+        <v>97.26511240005493</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1270,7 +1270,7 @@
         <v>2</v>
       </c>
       <c r="D20">
-        <v>99.98645782470703</v>
+        <v>99.99951124191284</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1281,7 +1281,7 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>99.99998807907104</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1292,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1325,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1336,7 +1336,7 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>100</v>
+        <v>99.99978542327881</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1380,7 +1380,7 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>99.99974966049194</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1402,7 +1402,7 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <v>99.99998807907104</v>
+        <v>99.99543428421021</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1435,7 +1435,7 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1454,10 +1454,10 @@
         <v>38</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>99.99848604202271</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1468,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1523,7 +1523,7 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <v>99.99991655349731</v>
+        <v>99.72549080848694</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1556,7 +1556,7 @@
         <v>2</v>
       </c>
       <c r="D46">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1578,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="D48">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1644,7 +1644,7 @@
         <v>2</v>
       </c>
       <c r="D54">
-        <v>84.04362201690674</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1655,7 +1655,7 @@
         <v>2</v>
       </c>
       <c r="D55">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1666,7 +1666,7 @@
         <v>2</v>
       </c>
       <c r="D56">
-        <v>99.99982118606567</v>
+        <v>99.96091723442078</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <v>99.99501705169678</v>
+        <v>99.9971866607666</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1699,7 +1699,7 @@
         <v>2</v>
       </c>
       <c r="D59">
-        <v>98.77257943153381</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1718,7 +1718,7 @@
         <v>62</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <v>100</v>
@@ -1732,7 +1732,7 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>99.94651675224304</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1743,7 +1743,7 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>100</v>
+        <v>99.99991655349731</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1751,10 +1751,10 @@
         <v>65</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64">
-        <v>99.99245405197144</v>
+        <v>99.98040795326233</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1809,7 +1809,7 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <v>100</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1820,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="D70">
-        <v>99.99833106994629</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1842,7 +1842,7 @@
         <v>2</v>
       </c>
       <c r="D72">
-        <v>99.99938011169434</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1853,7 +1853,7 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>99.99674558639526</v>
+        <v>99.99181032180786</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1908,7 +1908,7 @@
         <v>2</v>
       </c>
       <c r="D78">
-        <v>97.30775952339172</v>
+        <v>99.99961853027344</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1916,10 +1916,10 @@
         <v>80</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D79">
-        <v>99.99839067459106</v>
+        <v>84.98300909996033</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1930,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <v>99.9987006187439</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1941,7 +1941,7 @@
         <v>2</v>
       </c>
       <c r="D81">
-        <v>99.9997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1949,10 +1949,10 @@
         <v>83</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>99.99990463256836</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1974,7 +1974,7 @@
         <v>1</v>
       </c>
       <c r="D84">
-        <v>92.52040982246399</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2007,7 +2007,7 @@
         <v>2</v>
       </c>
       <c r="D87">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2015,10 +2015,10 @@
         <v>89</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88">
-        <v>90.89524745941162</v>
+        <v>53.71508002281189</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2026,10 +2026,10 @@
         <v>90</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89">
-        <v>99.98781681060791</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2037,10 +2037,10 @@
         <v>91</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D90">
-        <v>99.99903440475464</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2051,7 +2051,7 @@
         <v>2</v>
       </c>
       <c r="D91">
-        <v>99.9982476234436</v>
+        <v>100</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2062,7 +2062,7 @@
         <v>2</v>
       </c>
       <c r="D92">
-        <v>100</v>
+        <v>99.99669790267944</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2073,7 +2073,7 @@
         <v>2</v>
       </c>
       <c r="D93">
-        <v>99.99628067016602</v>
+        <v>99.89771842956543</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2084,7 +2084,7 @@
         <v>2</v>
       </c>
       <c r="D94">
-        <v>100</v>
+        <v>89.76674675941467</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2106,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="D96">
-        <v>99.99998807907104</v>
+        <v>99.99967813491821</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2128,7 +2128,7 @@
         <v>2</v>
       </c>
       <c r="D98">
-        <v>99.99974966049194</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2150,7 +2150,7 @@
         <v>2</v>
       </c>
       <c r="D100">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2161,7 +2161,7 @@
         <v>2</v>
       </c>
       <c r="D101">
-        <v>100</v>
+        <v>99.98487234115601</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2172,7 +2172,7 @@
         <v>2</v>
       </c>
       <c r="D102">
-        <v>99.85337257385254</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2227,7 +2227,7 @@
         <v>2</v>
       </c>
       <c r="D107">
-        <v>100</v>
+        <v>99.99212026596069</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2238,7 +2238,7 @@
         <v>2</v>
       </c>
       <c r="D108">
-        <v>100</v>
+        <v>99.99955892562866</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2249,7 +2249,7 @@
         <v>2</v>
       </c>
       <c r="D109">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2257,10 +2257,10 @@
         <v>111</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D110">
-        <v>99.99411106109619</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2271,7 +2271,7 @@
         <v>2</v>
       </c>
       <c r="D111">
-        <v>99.99972581863403</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2315,7 +2315,7 @@
         <v>2</v>
       </c>
       <c r="D115">
-        <v>99.99985694885254</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2323,10 +2323,10 @@
         <v>117</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D116">
-        <v>99.99997615814209</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2334,10 +2334,10 @@
         <v>118</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D117">
-        <v>97.88206219673157</v>
+        <v>99.99616146087646</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2348,7 +2348,7 @@
         <v>2</v>
       </c>
       <c r="D118">
-        <v>97.74078726768494</v>
+        <v>99.97789263725281</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2392,7 +2392,7 @@
         <v>2</v>
       </c>
       <c r="D122">
-        <v>99.99998807907104</v>
+        <v>99.99954700469971</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2414,7 +2414,7 @@
         <v>2</v>
       </c>
       <c r="D124">
-        <v>99.99992847442627</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2444,10 +2444,10 @@
         <v>128</v>
       </c>
       <c r="C127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D127">
-        <v>97.6487398147583</v>
+        <v>100</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2458,7 +2458,7 @@
         <v>2</v>
       </c>
       <c r="D128">
-        <v>99.99998807907104</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2480,7 +2480,7 @@
         <v>2</v>
       </c>
       <c r="D130">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2510,10 +2510,10 @@
         <v>134</v>
       </c>
       <c r="C133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D133">
-        <v>99.99991655349731</v>
+        <v>99.99511241912842</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2524,7 +2524,7 @@
         <v>2</v>
       </c>
       <c r="D134">
-        <v>99.99891519546509</v>
+        <v>100</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2535,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="D135">
-        <v>100</v>
+        <v>99.99905824661255</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2546,7 +2546,7 @@
         <v>2</v>
       </c>
       <c r="D136">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2590,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="D140">
-        <v>100</v>
+        <v>99.98816251754761</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2623,7 +2623,7 @@
         <v>2</v>
       </c>
       <c r="D143">
-        <v>100</v>
+        <v>99.99986886978149</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2634,7 +2634,7 @@
         <v>2</v>
       </c>
       <c r="D144">
-        <v>99.9998927116394</v>
+        <v>100</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2733,7 +2733,7 @@
         <v>2</v>
       </c>
       <c r="D153">
-        <v>99.99921321868896</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2755,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="D155">
-        <v>98.9899218082428</v>
+        <v>100</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2766,7 +2766,7 @@
         <v>2</v>
       </c>
       <c r="D156">
-        <v>99.99548196792603</v>
+        <v>100</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2777,7 +2777,7 @@
         <v>2</v>
       </c>
       <c r="D157">
-        <v>99.99963045120239</v>
+        <v>100</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2810,7 +2810,7 @@
         <v>2</v>
       </c>
       <c r="D160">
-        <v>87.50811219215393</v>
+        <v>100</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2818,10 +2818,10 @@
         <v>162</v>
       </c>
       <c r="C161">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D161">
-        <v>98.70291948318481</v>
+        <v>92.17342138290405</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2832,7 +2832,7 @@
         <v>2</v>
       </c>
       <c r="D162">
-        <v>99.99996423721313</v>
+        <v>100</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2843,7 +2843,7 @@
         <v>2</v>
       </c>
       <c r="D163">
-        <v>99.80314373970032</v>
+        <v>100</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2854,7 +2854,7 @@
         <v>2</v>
       </c>
       <c r="D164">
-        <v>64.85191583633423</v>
+        <v>95.80987691879272</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2876,7 +2876,7 @@
         <v>2</v>
       </c>
       <c r="D166">
-        <v>100</v>
+        <v>81.40982389450073</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2887,7 +2887,7 @@
         <v>2</v>
       </c>
       <c r="D167">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2898,7 +2898,7 @@
         <v>2</v>
       </c>
       <c r="D168">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2909,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="D169">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2920,7 +2920,7 @@
         <v>2</v>
       </c>
       <c r="D170">
-        <v>99.99974966049194</v>
+        <v>99.99955892562866</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2953,7 +2953,7 @@
         <v>2</v>
       </c>
       <c r="D173">
-        <v>99.99557733535767</v>
+        <v>100</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3008,7 +3008,7 @@
         <v>2</v>
       </c>
       <c r="D178">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3019,7 +3019,7 @@
         <v>2</v>
       </c>
       <c r="D179">
-        <v>100</v>
+        <v>99.9994158744812</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3041,7 +3041,7 @@
         <v>2</v>
       </c>
       <c r="D181">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -3071,10 +3071,10 @@
         <v>185</v>
       </c>
       <c r="C184">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D184">
-        <v>100</v>
+        <v>97.34569787979126</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3082,10 +3082,10 @@
         <v>186</v>
       </c>
       <c r="C185">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D185">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3093,10 +3093,10 @@
         <v>187</v>
       </c>
       <c r="C186">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D186">
-        <v>99.99964237213135</v>
+        <v>64.0005350112915</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3118,7 +3118,7 @@
         <v>2</v>
       </c>
       <c r="D188">
-        <v>99.99986886978149</v>
+        <v>100</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3126,10 +3126,10 @@
         <v>190</v>
       </c>
       <c r="C189">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D189">
-        <v>99.99990463256836</v>
+        <v>100</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3170,10 +3170,10 @@
         <v>194</v>
       </c>
       <c r="C193">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D193">
-        <v>78.27016711235046</v>
+        <v>100</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3206,7 +3206,7 @@
         <v>2</v>
       </c>
       <c r="D196">
-        <v>99.99994039535522</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3236,10 +3236,10 @@
         <v>200</v>
       </c>
       <c r="C199">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D199">
-        <v>89.12178874015808</v>
+        <v>99.99889135360718</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3250,7 +3250,7 @@
         <v>1</v>
       </c>
       <c r="D200">
-        <v>79.32512164115906</v>
+        <v>99.99468326568604</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3272,7 +3272,7 @@
         <v>2</v>
       </c>
       <c r="D202">
-        <v>99.98267292976379</v>
+        <v>100</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3291,10 +3291,10 @@
         <v>205</v>
       </c>
       <c r="C204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D204">
-        <v>54.62914705276489</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3316,7 +3316,7 @@
         <v>2</v>
       </c>
       <c r="D206">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3360,7 +3360,7 @@
         <v>2</v>
       </c>
       <c r="D210">
-        <v>99.99994039535522</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3371,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="D211">
-        <v>98.72542023658752</v>
+        <v>63.68331909179688</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3393,7 +3393,7 @@
         <v>2</v>
       </c>
       <c r="D213">
-        <v>99.9998927116394</v>
+        <v>99.99988079071045</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3404,7 +3404,7 @@
         <v>2</v>
       </c>
       <c r="D214">
-        <v>99.99996423721313</v>
+        <v>99.90843534469604</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3426,7 +3426,7 @@
         <v>2</v>
       </c>
       <c r="D216">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3434,10 +3434,10 @@
         <v>217</v>
       </c>
       <c r="C217">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D217">
-        <v>99.99959468841553</v>
+        <v>99.99675750732422</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3470,7 +3470,7 @@
         <v>1</v>
       </c>
       <c r="D220">
-        <v>87.21507787704468</v>
+        <v>100</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3478,7 +3478,7 @@
         <v>221</v>
       </c>
       <c r="C221">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D221">
         <v>100</v>
@@ -3492,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="D222">
-        <v>99.98846054077148</v>
+        <v>100</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3503,7 +3503,7 @@
         <v>2</v>
       </c>
       <c r="D223">
-        <v>100</v>
+        <v>99.99940395355225</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3514,7 +3514,7 @@
         <v>1</v>
       </c>
       <c r="D224">
-        <v>99.99992847442627</v>
+        <v>100</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3525,7 +3525,7 @@
         <v>1</v>
       </c>
       <c r="D225">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3536,7 +3536,7 @@
         <v>1</v>
       </c>
       <c r="D226">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3544,10 +3544,10 @@
         <v>227</v>
       </c>
       <c r="C227">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D227">
-        <v>68.4438943862915</v>
+        <v>100</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3566,10 +3566,10 @@
         <v>229</v>
       </c>
       <c r="C229">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D229">
-        <v>100</v>
+        <v>99.9998927116394</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3580,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="D230">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3591,7 +3591,7 @@
         <v>1</v>
       </c>
       <c r="D231">
-        <v>99.99896287918091</v>
+        <v>100</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3610,10 +3610,10 @@
         <v>233</v>
       </c>
       <c r="C233">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D233">
-        <v>99.72967505455017</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>